<commit_message>
Added CAD Model and Partslist
</commit_message>
<xml_diff>
--- a/PCB/CycleOpsPro300toANTPlus_V1.0_Parts_List.xlsx
+++ b/PCB/CycleOpsPro300toANTPlus_V1.0_Parts_List.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive Matt\Personal Backup\CycleOps Pro 300PT Drive\GIt Files\CycleOpsPro300PTtoANTPlus\PCB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive Matt\Personal Backup\CycleOps Pro 300PT Drive\Git Files\CycleOpsPro300PTtoANTPlus\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="110">
   <si>
     <t>Part</t>
   </si>
@@ -325,6 +325,30 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Parts</t>
+  </si>
+  <si>
+    <t>Power Switch</t>
+  </si>
+  <si>
+    <t>108-0041-EVX</t>
+  </si>
+  <si>
+    <t>Mountain Switch</t>
+  </si>
+  <si>
+    <t>Toggle Switches SPST OFF-ON</t>
+  </si>
+  <si>
+    <t>Reset Switch</t>
+  </si>
+  <si>
+    <t>103-1013-EVX</t>
+  </si>
+  <si>
+    <t>Pushbutton Switches METAL BODY BLK</t>
   </si>
 </sst>
 </file>
@@ -467,7 +491,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -645,6 +669,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -808,8 +838,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1131,10 +1162,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M33"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1216,7 +1247,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B3" t="s">
@@ -1236,7 +1267,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B4" t="s">
@@ -1256,7 +1287,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B5" t="s">
@@ -1276,7 +1307,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B6" t="s">
@@ -1296,7 +1327,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B7" t="s">
@@ -1350,7 +1381,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B10" t="s">
@@ -1376,7 +1407,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B11" t="s">
@@ -1450,7 +1481,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B15" t="s">
@@ -1465,12 +1496,12 @@
       <c r="E15" t="s">
         <v>57</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B16" t="s">
@@ -1490,7 +1521,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B17">
@@ -1510,7 +1541,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B18">
@@ -1530,7 +1561,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B19">
@@ -1550,7 +1581,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B20" t="s">
@@ -1570,7 +1601,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B21" t="s">
@@ -1585,12 +1616,12 @@
       <c r="E21" t="s">
         <v>57</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B22" t="s">
@@ -1605,12 +1636,12 @@
       <c r="E22" t="s">
         <v>57</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B23" t="s">
@@ -1630,7 +1661,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>70</v>
       </c>
       <c r="B24">
@@ -1650,7 +1681,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B25" t="s">
@@ -1665,12 +1696,12 @@
       <c r="E25" t="s">
         <v>57</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F25" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B26" t="s">
@@ -1690,7 +1721,7 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B27" t="s">
@@ -1761,7 +1792,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B31" t="s">
@@ -1807,7 +1838,7 @@
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B33" t="s">
@@ -1841,7 +1872,41 @@
         <v>96</v>
       </c>
     </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" t="s">
+        <v>104</v>
+      </c>
+      <c r="D36" t="s">
+        <v>105</v>
+      </c>
+      <c r="E36" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37" t="s">
+        <v>105</v>
+      </c>
+      <c r="E37" t="s">
+        <v>109</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update to Parts List
</commit_message>
<xml_diff>
--- a/PCB/CycleOpsPro300toANTPlus_V1.0_Parts_List.xlsx
+++ b/PCB/CycleOpsPro300toANTPlus_V1.0_Parts_List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="120">
   <si>
     <t>Part</t>
   </si>
@@ -363,6 +363,24 @@
   </si>
   <si>
     <t>Project Case</t>
+  </si>
+  <si>
+    <t>Molex Micro-Fit 4 Circuit plug Housing</t>
+  </si>
+  <si>
+    <t>Molex Micro-Fit Pins</t>
+  </si>
+  <si>
+    <t>538-43020-0400</t>
+  </si>
+  <si>
+    <t>538-43031-0007</t>
+  </si>
+  <si>
+    <t>Battery 14500 3.7V Li-Ion</t>
+  </si>
+  <si>
+    <t>http://www.dx.com/p/trustfire-protected-14500-3-7v-900mah-lithium-batteries-2-pack-blue-19626</t>
   </si>
 </sst>
 </file>
@@ -1190,15 +1208,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="46.5703125" customWidth="1"/>
     <col min="5" max="5" width="26.7109375" customWidth="1"/>
@@ -1836,14 +1854,39 @@
         <v>112</v>
       </c>
     </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E34" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F32" r:id="rId1"/>
     <hyperlink ref="F29" r:id="rId2"/>
     <hyperlink ref="F24" r:id="rId3"/>
     <hyperlink ref="F33" r:id="rId4"/>
+    <hyperlink ref="F36" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated CAD Model. Minor corrections to schematic. Updated BOM Parts List.
Signed-off-by: Matt W <mwasserman@gmail.com>
</commit_message>
<xml_diff>
--- a/PCB/CycleOpsPro300toANTPlus_V1.0_Parts_List.xlsx
+++ b/PCB/CycleOpsPro300toANTPlus_V1.0_Parts_List.xlsx
@@ -14,12 +14,15 @@
   <sheets>
     <sheet name="CycleOpsPro300toANTPlus_V1.0_Pa" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CycleOpsPro300toANTPlus_V1.0_Pa!$A$1:$H$29</definedName>
+  </definedNames>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="114">
   <si>
     <t>Part</t>
   </si>
@@ -60,9 +63,6 @@
     <t>Capacitor</t>
   </si>
   <si>
-    <t>C2</t>
-  </si>
-  <si>
     <t>1.0uF</t>
   </si>
   <si>
@@ -72,12 +72,6 @@
     <t>2.2uF</t>
   </si>
   <si>
-    <t>C4</t>
-  </si>
-  <si>
-    <t>C5</t>
-  </si>
-  <si>
     <t>D1</t>
   </si>
   <si>
@@ -141,24 +135,6 @@
     <t>Resistor</t>
   </si>
   <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>10.0K</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>R5</t>
-  </si>
-  <si>
-    <t>R6</t>
-  </si>
-  <si>
     <t>10K</t>
   </si>
   <si>
@@ -171,27 +147,15 @@
     <t>1.0M</t>
   </si>
   <si>
-    <t>R9</t>
-  </si>
-  <si>
-    <t>R10</t>
-  </si>
-  <si>
     <t>R11</t>
   </si>
   <si>
     <t>4.7M</t>
   </si>
   <si>
-    <t>R12</t>
-  </si>
-  <si>
     <t>4.7K</t>
   </si>
   <si>
-    <t>R13</t>
-  </si>
-  <si>
     <t>U$1</t>
   </si>
   <si>
@@ -271,10 +235,6 @@
   </si>
   <si>
     <t>Mouser Part #</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-103-1013-EVX</t>
   </si>
   <si>
     <t>581-06036D475MAT4A</t>
@@ -353,9 +313,6 @@
     <t>621-AP2112K-3.3TRG1</t>
   </si>
   <si>
-    <t>595-TPS78223DDCR</t>
-  </si>
-  <si>
     <t>OLED Display</t>
   </si>
   <si>
@@ -381,6 +338,33 @@
   </si>
   <si>
     <t>http://www.dx.com/p/trustfire-protected-14500-3-7v-900mah-lithium-batteries-2-pack-blue-19626</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>R3, R4</t>
+  </si>
+  <si>
+    <t>R5, R10</t>
+  </si>
+  <si>
+    <t>C2, C4, C5</t>
+  </si>
+  <si>
+    <t>R2, R6, R9</t>
+  </si>
+  <si>
+    <t>R12, R13</t>
+  </si>
+  <si>
+    <t>TPS78001DDCR</t>
+  </si>
+  <si>
+    <t>595-TPS78001DDCR</t>
   </si>
 </sst>
 </file>
@@ -1208,10 +1192,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1224,7 +1208,7 @@
     <col min="7" max="7" width="28.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1238,61 +1222,60 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="F1" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="G1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2">
+        <f>6.88+1.85</f>
+        <v>8.73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H3">
+        <f>5.73/2</f>
+        <v>2.8650000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -1300,19 +1283,22 @@
       <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>87</v>
+      <c r="E4" t="s">
+        <v>71</v>
       </c>
       <c r="G4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>17</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>11</v>
@@ -1321,18 +1307,21 @@
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="G5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -1340,551 +1329,481 @@
       <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="E6" t="s">
-        <v>86</v>
+      <c r="E6" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="G6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="D7" t="s">
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>75</v>
+      </c>
+      <c r="G8" t="s">
         <v>23</v>
       </c>
-      <c r="E7" t="s">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>76</v>
+      </c>
+      <c r="G9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H10">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H11">
+        <f>0.23*4</f>
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>96</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H12">
+        <v>11.95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" t="s">
+        <v>60</v>
+      </c>
+      <c r="G13" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13">
+        <v>2.83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>98</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H14">
+        <f>4.5/5</f>
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" t="s">
+        <v>77</v>
+      </c>
+      <c r="G15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" t="s">
+        <v>79</v>
+      </c>
+      <c r="G16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" t="s">
+        <v>86</v>
+      </c>
+      <c r="G17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" t="s">
+        <v>87</v>
+      </c>
+      <c r="G18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" t="s">
+        <v>35</v>
+      </c>
+      <c r="D19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20">
+        <v>200</v>
+      </c>
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" t="s">
+        <v>80</v>
+      </c>
+      <c r="G20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B21">
+        <v>470</v>
+      </c>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" t="s">
+        <v>36</v>
+      </c>
+      <c r="E21" t="s">
+        <v>81</v>
+      </c>
+      <c r="G21" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" t="s">
+        <v>83</v>
+      </c>
+      <c r="G22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" t="s">
+        <v>85</v>
+      </c>
+      <c r="G23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G24" t="s">
+        <v>64</v>
+      </c>
+      <c r="H24">
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" t="s">
+        <v>89</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" t="s">
-        <v>89</v>
-      </c>
-      <c r="G8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" t="s">
-        <v>90</v>
-      </c>
-      <c r="G9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="G25" t="s">
+        <v>45</v>
+      </c>
+      <c r="H25">
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" t="s">
+        <v>92</v>
+      </c>
+      <c r="E26" t="s">
         <v>91</v>
       </c>
-      <c r="G10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" t="s">
-        <v>92</v>
-      </c>
-      <c r="C11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="G26" t="s">
+        <v>47</v>
+      </c>
+      <c r="H26">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" t="s">
+        <v>94</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13">
-        <v>200</v>
-      </c>
-      <c r="C13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" t="s">
-        <v>94</v>
-      </c>
-      <c r="G13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14">
-        <v>200</v>
-      </c>
-      <c r="C14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" t="s">
-        <v>94</v>
-      </c>
-      <c r="G14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15">
-        <v>470</v>
-      </c>
-      <c r="C15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="G27" t="s">
+        <v>49</v>
+      </c>
+      <c r="H27">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" t="s">
         <v>95</v>
       </c>
-      <c r="G15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" t="s">
-        <v>39</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" t="s">
-        <v>96</v>
-      </c>
-      <c r="C17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" t="s">
-        <v>97</v>
-      </c>
-      <c r="G17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" t="s">
-        <v>99</v>
-      </c>
-      <c r="G18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" t="s">
-        <v>39</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20">
-        <v>470</v>
-      </c>
-      <c r="C20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" t="s">
-        <v>95</v>
-      </c>
-      <c r="G20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="G28" t="s">
         <v>53</v>
       </c>
-      <c r="C21" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" t="s">
-        <v>100</v>
-      </c>
-      <c r="G21" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="H28">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" t="s">
-        <v>39</v>
-      </c>
-      <c r="E22" t="s">
-        <v>101</v>
-      </c>
-      <c r="G22" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="B29" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E29" t="s">
+        <v>113</v>
+      </c>
+      <c r="G29" t="s">
         <v>56</v>
       </c>
-      <c r="B23" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" t="s">
-        <v>39</v>
-      </c>
-      <c r="E23" t="s">
-        <v>101</v>
-      </c>
-      <c r="G23" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B24" t="s">
-        <v>104</v>
-      </c>
-      <c r="D24" t="s">
-        <v>103</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G24" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B25" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25" t="s">
-        <v>60</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="H29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
         <v>106</v>
       </c>
-      <c r="E25" t="s">
-        <v>105</v>
-      </c>
-      <c r="G25" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B26" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" t="s">
-        <v>63</v>
-      </c>
-      <c r="D26" t="s">
-        <v>108</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G26" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B27" t="s">
-        <v>65</v>
-      </c>
-      <c r="C27" t="s">
-        <v>63</v>
-      </c>
-      <c r="D27" t="s">
-        <v>67</v>
-      </c>
-      <c r="E27" t="s">
-        <v>109</v>
-      </c>
-      <c r="G27" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B28" t="s">
-        <v>69</v>
-      </c>
-      <c r="C28" t="s">
-        <v>70</v>
-      </c>
-      <c r="D28" t="s">
-        <v>71</v>
-      </c>
-      <c r="E28" t="s">
-        <v>110</v>
-      </c>
-      <c r="G28" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B29" t="s">
-        <v>79</v>
-      </c>
-      <c r="C29" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" t="s">
-        <v>7</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G29" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C30" t="s">
-        <v>74</v>
-      </c>
-      <c r="D30" t="s">
-        <v>75</v>
-      </c>
-      <c r="E30" t="s">
-        <v>73</v>
-      </c>
-      <c r="G30" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="C31" t="s">
-        <v>74</v>
-      </c>
-      <c r="D31" t="s">
-        <v>78</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="G31" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>113</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>111</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E34" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>119</v>
+      <c r="H32">
+        <f>SUM(H2:H29)</f>
+        <v>49.924999999999997</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H29">
+    <sortState ref="A2:H29">
+      <sortCondition ref="A1:A29"/>
+    </sortState>
+  </autoFilter>
   <hyperlinks>
-    <hyperlink ref="F32" r:id="rId1"/>
-    <hyperlink ref="F29" r:id="rId2"/>
-    <hyperlink ref="F24" r:id="rId3"/>
-    <hyperlink ref="F33" r:id="rId4"/>
-    <hyperlink ref="F36" r:id="rId5"/>
+    <hyperlink ref="F14" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId2"/>
+    <hyperlink ref="F25" r:id="rId3"/>
+    <hyperlink ref="F12" r:id="rId4"/>
+    <hyperlink ref="F3" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>

</xml_diff>